<commit_message>
Aggiunti nomi agli assi cartesiani
</commit_message>
<xml_diff>
--- a/progetto/final_report.xlsx
+++ b/progetto/final_report.xlsx
@@ -116,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -130,15 +130,8 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -176,17 +169,7 @@
           <a:bodyPr/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" spc="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
               <a:rPr/>
@@ -244,7 +227,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>local_emi</c:v>
+                  <c:v>Laptop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -307,21 +290,21 @@
             <c:numRef>
               <c:f>'Task 1'!$B$50:$B$54</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0">
                   <c:v>3.14</c:v>
                 </c:pt>
-                <c:pt idx="1" formatCode="0.00">
+                <c:pt idx="1">
                   <c:v>5.05</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="00.00">
+                <c:pt idx="2">
                   <c:v>12.12</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="00.00">
+                <c:pt idx="3">
                   <c:v>40.55</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="00.00">
+                <c:pt idx="4">
                   <c:v>75.58</c:v>
                 </c:pt>
               </c:numCache>
@@ -338,7 +321,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>local_gio</c:v>
+                  <c:v>Desktop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -432,7 +415,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>emr</c:v>
+                  <c:v>Emr</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -517,19 +500,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls>
-          <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
-        </c:dLbls>
-        <c:axId val="2140841523"/>
-        <c:axId val="2140841524"/>
+        <c:axId val="2140841569"/>
+        <c:axId val="2140841570"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2140841523"/>
+        <c:axId val="2140841569"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200.000000"/>
@@ -553,6 +528,67 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Dataset %</a:t>
+                </a:r>
+                <a:endParaRPr b="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr bwMode="auto">
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -591,12 +627,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140841524"/>
+        <c:crossAx val="2140841570"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2140841524"/>
+        <c:axId val="2140841570"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -619,6 +655,34 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1"/>
+                  <a:t>Time (S)</a:t>
+                </a:r>
+                <a:endParaRPr b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:txPr>
+            <a:bodyPr/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr b="0"/>
+              </a:pPr>
+              <a:endParaRPr/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -657,7 +721,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140841523"/>
+        <c:crossAx val="2140841569"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -710,8 +774,8 @@
   </c:chart>
   <c:spPr bwMode="auto">
     <a:xfrm>
-      <a:off x="6300786" y="8986836"/>
-      <a:ext cx="4552949" cy="2643187"/>
+      <a:off x="6119810" y="9596435"/>
+      <a:ext cx="4552948" cy="2900362"/>
     </a:xfrm>
     <a:prstGeom prst="rect">
       <a:avLst/>
@@ -777,7 +841,7 @@
             </a:pPr>
             <a:r>
               <a:rPr/>
-              <a:t>Spark-core</a:t>
+              <a:t>Spark</a:t>
             </a:r>
             <a:endParaRPr/>
           </a:p>
@@ -831,7 +895,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>local_emi</c:v>
+                  <c:v>Laptop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -925,7 +989,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>local_gio</c:v>
+                  <c:v>Desktop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1019,7 +1083,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>emr</c:v>
+                  <c:v>Emr</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1104,19 +1168,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls>
-          <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
-        </c:dLbls>
-        <c:axId val="2140841537"/>
-        <c:axId val="2140841538"/>
+        <c:axId val="2140841573"/>
+        <c:axId val="2140841574"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2140841537"/>
+        <c:axId val="2140841573"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200.000000"/>
@@ -1140,6 +1196,34 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr/>
+                  <a:t>Dataset %</a:t>
+                </a:r>
+                <a:endParaRPr/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:txPr>
+            <a:bodyPr/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr/>
+              </a:pPr>
+              <a:endParaRPr/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1178,12 +1262,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140841538"/>
+        <c:crossAx val="2140841574"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2140841538"/>
+        <c:axId val="2140841574"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1206,6 +1290,34 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr/>
+                  <a:t>Time (S)</a:t>
+                </a:r>
+                <a:endParaRPr/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:txPr>
+            <a:bodyPr/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr/>
+              </a:pPr>
+              <a:endParaRPr/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1244,7 +1356,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140841537"/>
+        <c:crossAx val="2140841573"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1297,8 +1409,8 @@
   </c:chart>
   <c:spPr bwMode="auto">
     <a:xfrm>
-      <a:off x="11653836" y="8896349"/>
-      <a:ext cx="4552949" cy="2824162"/>
+      <a:off x="11006135" y="9596435"/>
+      <a:ext cx="4552949" cy="2900362"/>
     </a:xfrm>
     <a:prstGeom prst="rect">
       <a:avLst/>
@@ -1418,7 +1530,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>local_emi</c:v>
+                  <c:v>Laptop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1512,7 +1624,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>local_gio</c:v>
+                  <c:v>Desktop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1606,7 +1718,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>emr</c:v>
+                  <c:v>Emr</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1691,19 +1803,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls>
-          <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
-        </c:dLbls>
-        <c:axId val="2140841539"/>
-        <c:axId val="2140841540"/>
+        <c:axId val="2140841571"/>
+        <c:axId val="2140841572"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2140841539"/>
+        <c:axId val="2140841571"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200.000000"/>
@@ -1727,6 +1831,38 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Dataset %</a:t>
+                </a:r>
+                <a:endParaRPr/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:txPr>
+            <a:bodyPr/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr/>
+              </a:pPr>
+              <a:endParaRPr/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1765,12 +1901,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140841540"/>
+        <c:crossAx val="2140841572"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2140841540"/>
+        <c:axId val="2140841572"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1793,6 +1929,34 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr/>
+                  <a:t>Time (S)</a:t>
+                </a:r>
+                <a:endParaRPr/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:txPr>
+            <a:bodyPr/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr/>
+              </a:pPr>
+              <a:endParaRPr/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="00.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1831,7 +1995,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140841539"/>
+        <c:crossAx val="2140841571"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1884,8 +2048,8 @@
   </c:chart>
   <c:spPr bwMode="auto">
     <a:xfrm>
-      <a:off x="8253411" y="5314949"/>
-      <a:ext cx="4652962" cy="2805111"/>
+      <a:off x="8558210" y="6505573"/>
+      <a:ext cx="4652962" cy="2881311"/>
     </a:xfrm>
     <a:prstGeom prst="rect">
       <a:avLst/>
@@ -1947,17 +2111,7 @@
           <a:bodyPr/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" spc="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
               <a:rPr/>
@@ -2015,7 +2169,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>local_emi</c:v>
+                  <c:v>Laptop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2109,7 +2263,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>local_gio</c:v>
+                  <c:v>Desktop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2203,7 +2357,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>emr</c:v>
+                  <c:v>Emr</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2288,19 +2442,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls>
-          <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
-        </c:dLbls>
-        <c:axId val="2140841561"/>
-        <c:axId val="2140841562"/>
+        <c:axId val="2140841575"/>
+        <c:axId val="2140841576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2140841561"/>
+        <c:axId val="2140841575"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200.000000"/>
@@ -2324,6 +2470,34 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr/>
+                  <a:t>Dataset %</a:t>
+                </a:r>
+                <a:endParaRPr/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:txPr>
+            <a:bodyPr/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr/>
+              </a:pPr>
+              <a:endParaRPr/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2362,12 +2536,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140841562"/>
+        <c:crossAx val="2140841576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2140841562"/>
+        <c:axId val="2140841576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2390,6 +2564,34 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr/>
+                  <a:t>Time (S)</a:t>
+                </a:r>
+                <a:endParaRPr/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:txPr>
+            <a:bodyPr/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr/>
+              </a:pPr>
+              <a:endParaRPr/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2428,7 +2630,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140841561"/>
+        <c:crossAx val="2140841575"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2481,8 +2683,8 @@
   </c:chart>
   <c:spPr bwMode="auto">
     <a:xfrm>
-      <a:off x="5410198" y="8713786"/>
-      <a:ext cx="4565649" cy="2628900"/>
+      <a:off x="6088060" y="9586910"/>
+      <a:ext cx="4554536" cy="2890838"/>
     </a:xfrm>
     <a:prstGeom prst="rect">
       <a:avLst/>
@@ -2544,17 +2746,7 @@
           <a:bodyPr/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" spc="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
               <a:rPr/>
@@ -2609,6 +2801,12 @@
           <c:tx>
             <c:strRef>
               <c:f>'Task 2'!$B$57</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Laptop</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr bwMode="auto">
@@ -2645,11 +2843,48 @@
           <c:xVal>
             <c:strRef>
               <c:f>'Task 2'!$A$58:$A$62</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>'Task 2'!$B$58:$B$62</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8.89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49.82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>204.76</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>417.1</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
@@ -2660,6 +2895,12 @@
           <c:tx>
             <c:strRef>
               <c:f>'Task 2'!$C$57</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Desktop</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr bwMode="auto">
@@ -2696,11 +2937,48 @@
           <c:xVal>
             <c:strRef>
               <c:f>'Task 2'!$A$58:$A$62</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>'Task 2'!$C$58:$C$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.61</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44.84</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>89.97</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
@@ -2711,6 +2989,12 @@
           <c:tx>
             <c:strRef>
               <c:f>'Task 2'!$D$57</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Emr</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr bwMode="auto">
@@ -2747,30 +3031,60 @@
           <c:xVal>
             <c:strRef>
               <c:f>'Task 2'!$A$58:$A$62</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>'Task 2'!$D$58:$D$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>26.09</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38.12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>127.29</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>225.02</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls>
-          <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
-        </c:dLbls>
-        <c:axId val="2140841551"/>
-        <c:axId val="2140841552"/>
+        <c:axId val="2140841581"/>
+        <c:axId val="2140841582"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2140841551"/>
+        <c:axId val="2140841581"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="200.000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2791,71 +3105,57 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr bwMode="auto">
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-                <a:ea typeface="Arial"/>
-                <a:cs typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2140841552"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="2140841552"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr>
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Dataset %</a:t>
+                </a:r>
+                <a:endParaRPr/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr bwMode="auto">
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
             <a:noFill/>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2894,7 +3194,128 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140841551"/>
+        <c:crossAx val="2140841582"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2140841582"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr bwMode="auto">
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Time (S)</a:t>
+                </a:r>
+                <a:endParaRPr b="1">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr bwMode="auto">
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr bwMode="auto">
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2140841581"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2947,8 +3368,8 @@
   </c:chart>
   <c:spPr bwMode="auto">
     <a:xfrm>
-      <a:off x="10277473" y="8713786"/>
-      <a:ext cx="4565649" cy="2628900"/>
+      <a:off x="10980735" y="9586910"/>
+      <a:ext cx="4554536" cy="2890838"/>
     </a:xfrm>
     <a:prstGeom prst="rect">
       <a:avLst/>
@@ -3010,17 +3431,7 @@
           <a:bodyPr/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" spc="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
               <a:rPr/>
@@ -3078,7 +3489,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>local_emi</c:v>
+                  <c:v>Laptop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3172,7 +3583,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>local_gio</c:v>
+                  <c:v>Desktop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3266,7 +3677,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>emr</c:v>
+                  <c:v>Emr</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3351,19 +3762,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls>
-          <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
-        </c:dLbls>
-        <c:axId val="2140841559"/>
-        <c:axId val="2140841560"/>
+        <c:axId val="2140841577"/>
+        <c:axId val="2140841578"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2140841559"/>
+        <c:axId val="2140841577"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200.000000"/>
@@ -3387,6 +3790,34 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr/>
+                  <a:t>Dataset %</a:t>
+                </a:r>
+                <a:endParaRPr/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:txPr>
+            <a:bodyPr/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr/>
+              </a:pPr>
+              <a:endParaRPr/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3425,12 +3856,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140841560"/>
+        <c:crossAx val="2140841578"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2140841560"/>
+        <c:axId val="2140841578"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3453,6 +3884,34 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr/>
+                  <a:t>Time (S)</a:t>
+                </a:r>
+                <a:endParaRPr/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:txPr>
+            <a:bodyPr/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr/>
+              </a:pPr>
+              <a:endParaRPr/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="00.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3491,7 +3950,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140841559"/>
+        <c:crossAx val="2140841577"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3544,8 +4003,8 @@
   </c:chart>
   <c:spPr bwMode="auto">
     <a:xfrm>
-      <a:off x="7431086" y="5140324"/>
-      <a:ext cx="4564062" cy="2628899"/>
+      <a:off x="8542335" y="6534149"/>
+      <a:ext cx="4551361" cy="2876548"/>
     </a:xfrm>
     <a:prstGeom prst="rect">
       <a:avLst/>
@@ -7101,16 +7560,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>52386</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>176211</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4760</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>4760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>338135</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>290509</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>9523</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7120,8 +7579,8 @@
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6300786" y="8986836"/>
-        <a:ext cx="4552949" cy="2643187"/>
+        <a:off x="6119810" y="9596435"/>
+        <a:ext cx="4552948" cy="2900362"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7133,16 +7592,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>528636</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>14285</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>4760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>204785</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>300034</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>9523</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7152,8 +7611,8 @@
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11653836" y="8896349"/>
-        <a:ext cx="4552949" cy="2824162"/>
+        <a:off x="11006135" y="9596435"/>
+        <a:ext cx="4552949" cy="2900362"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7165,16 +7624,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>176211</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>4760</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>171448</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>561973</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>14286</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>390522</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>157160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7184,8 +7643,8 @@
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8253411" y="5314949"/>
-        <a:ext cx="4652962" cy="2805111"/>
+        <a:off x="8558210" y="6505573"/>
+        <a:ext cx="4652962" cy="2881311"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7202,16 +7661,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>306386</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>157161</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>601660</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>176210</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>593723</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>166686</xdr:rowOff>
+      <xdr:colOff>279397</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7221,8 +7680,8 @@
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5410198" y="8713786"/>
-        <a:ext cx="4565649" cy="2628900"/>
+        <a:off x="6088060" y="9586910"/>
+        <a:ext cx="4554536" cy="2890838"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7235,15 +7694,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>284161</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>157161</xdr:rowOff>
+      <xdr:colOff>7935</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>176210</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>571498</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>166686</xdr:rowOff>
+      <xdr:colOff>295272</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7253,8 +7712,8 @@
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10277473" y="8713786"/>
-        <a:ext cx="4565649" cy="2628900"/>
+        <a:off x="10980735" y="9586910"/>
+        <a:ext cx="4554536" cy="2890838"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7266,16 +7725,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>493711</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>7935</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>168273</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:colOff>292097</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>180973</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7285,8 +7744,8 @@
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7431086" y="5140324"/>
-        <a:ext cx="4564062" cy="2628899"/>
+        <a:off x="8542335" y="6534149"/>
+        <a:ext cx="4551361" cy="2876548"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8473,7 +8932,7 @@
       <c r="C49" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E49" t="s">
@@ -8505,10 +8964,10 @@
       <c r="E50" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F50" s="8" t="s">
+      <c r="F50" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G50" s="8" t="s">
+      <c r="G50" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -8529,15 +8988,15 @@
         <v>30.050000000000001</v>
       </c>
       <c r="E51" s="3">
-        <f>(B51/B50)/(A51/A50)</f>
+        <f t="shared" ref="E51:E70" si="3">(B51/B50)/(A51/A50)</f>
         <v>0.321656050955414</v>
       </c>
       <c r="F51" s="3">
-        <f>(C51/C50)/(A51/A50)</f>
+        <f t="shared" ref="F51:F70" si="4">(C51/C50)/(A51/A50)</f>
         <v>0.28755364806866951</v>
       </c>
       <c r="G51" s="3">
-        <f>(D51/D50)/(A51/A50)</f>
+        <f t="shared" ref="G51:G69" si="5">(D51/D50)/(A51/A50)</f>
         <v>0.1835114503816794</v>
       </c>
     </row>
@@ -8558,15 +9017,15 @@
         <v>33</v>
       </c>
       <c r="E52" s="3">
-        <f>(B52/B51)/(A52/A51)</f>
+        <f t="shared" si="3"/>
         <v>0.59999999999999998</v>
       </c>
       <c r="F52" s="3">
-        <f>(C52/C51)/(A52/A51)</f>
+        <f t="shared" si="4"/>
         <v>0.39626865671641787</v>
       </c>
       <c r="G52" s="3">
-        <f>(D52/D51)/(A52/A51)</f>
+        <f t="shared" si="5"/>
         <v>0.27454242928452577</v>
       </c>
     </row>
@@ -8579,7 +9038,7 @@
         <v>40.549999999999997</v>
       </c>
       <c r="C53" s="1">
-        <f t="shared" ref="C53:C54" si="3">D10</f>
+        <f t="shared" ref="C53:C54" si="6">D10</f>
         <v>19.370000000000001</v>
       </c>
       <c r="D53" s="1">
@@ -8587,15 +9046,15 @@
         <v>106.61</v>
       </c>
       <c r="E53" s="3">
-        <f>(B53/B52)/(A53/A52)</f>
+        <f t="shared" si="3"/>
         <v>0.66914191419141911</v>
       </c>
       <c r="F53" s="3">
-        <f>(C53/C52)/(A53/A52)</f>
+        <f t="shared" si="4"/>
         <v>0.72956685499058394</v>
       </c>
       <c r="G53" s="3">
-        <f>(D53/D52)/(A53/A52)</f>
+        <f t="shared" si="5"/>
         <v>0.6461212121212121</v>
       </c>
     </row>
@@ -8608,7 +9067,7 @@
         <v>75.579999999999998</v>
       </c>
       <c r="C54" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>35.409999999999997</v>
       </c>
       <c r="D54" s="1">
@@ -8616,15 +9075,15 @@
         <v>187.49000000000001</v>
       </c>
       <c r="E54" s="3">
-        <f>(B54/B53)/(A54/A53)</f>
+        <f t="shared" si="3"/>
         <v>0.93193588162762031</v>
       </c>
       <c r="F54" s="3">
-        <f>(C54/C53)/(A54/A53)</f>
+        <f t="shared" si="4"/>
         <v>0.91404233350542063</v>
       </c>
       <c r="G54" s="3">
-        <f>(D54/D53)/(A54/A53)</f>
+        <f t="shared" si="5"/>
         <v>0.87932651721226907</v>
       </c>
     </row>
@@ -8674,15 +9133,15 @@
         <v>1</v>
       </c>
       <c r="B58" s="3">
-        <f t="shared" ref="B58:B62" si="4">D17</f>
+        <f t="shared" ref="B58:B62" si="7">D17</f>
         <v>6.5999999999999996</v>
       </c>
       <c r="C58">
-        <f t="shared" ref="C58:C62" si="5">D22</f>
+        <f t="shared" ref="C58:C62" si="8">D22</f>
         <v>4.4900000000000002</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" ref="D58:D62" si="6">D27</f>
+        <f t="shared" ref="D58:D62" si="9">D27</f>
         <v>27.870000000000001</v>
       </c>
       <c r="E58" s="1" t="s">
@@ -8700,27 +9159,27 @@
         <v>5</v>
       </c>
       <c r="B59" s="3">
+        <f t="shared" si="7"/>
+        <v>6.6200000000000001</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="8"/>
+        <v>5.6699999999999999</v>
+      </c>
+      <c r="D59" s="1">
+        <f t="shared" si="9"/>
+        <v>27.23</v>
+      </c>
+      <c r="E59" s="3">
+        <f t="shared" si="3"/>
+        <v>0.20060606060606062</v>
+      </c>
+      <c r="F59" s="3">
         <f t="shared" si="4"/>
-        <v>6.6200000000000001</v>
-      </c>
-      <c r="C59">
+        <v>0.25256124721603562</v>
+      </c>
+      <c r="G59" s="3">
         <f t="shared" si="5"/>
-        <v>5.6699999999999999</v>
-      </c>
-      <c r="D59" s="1">
-        <f t="shared" si="6"/>
-        <v>27.23</v>
-      </c>
-      <c r="E59" s="3">
-        <f>(B59/B58)/(A59/A58)</f>
-        <v>0.20060606060606062</v>
-      </c>
-      <c r="F59" s="3">
-        <f>(C59/C58)/(A59/A58)</f>
-        <v>0.25256124721603562</v>
-      </c>
-      <c r="G59" s="3">
-        <f>(D59/D58)/(A59/A58)</f>
         <v>0.19540724793684966</v>
       </c>
     </row>
@@ -8729,27 +9188,27 @@
         <v>20</v>
       </c>
       <c r="B60" s="3">
+        <f t="shared" si="7"/>
+        <v>14.15</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="8"/>
+        <v>7.9400000000000004</v>
+      </c>
+      <c r="D60" s="1">
+        <f t="shared" si="9"/>
+        <v>31.960000000000001</v>
+      </c>
+      <c r="E60" s="3">
+        <f t="shared" si="3"/>
+        <v>0.53436555891238668</v>
+      </c>
+      <c r="F60" s="3">
         <f t="shared" si="4"/>
-        <v>14.15</v>
-      </c>
-      <c r="C60">
+        <v>0.35008818342151676</v>
+      </c>
+      <c r="G60" s="3">
         <f t="shared" si="5"/>
-        <v>7.9400000000000004</v>
-      </c>
-      <c r="D60" s="1">
-        <f t="shared" si="6"/>
-        <v>31.960000000000001</v>
-      </c>
-      <c r="E60" s="3">
-        <f>(B60/B59)/(A60/A59)</f>
-        <v>0.53436555891238668</v>
-      </c>
-      <c r="F60" s="3">
-        <f>(C60/C59)/(A60/A59)</f>
-        <v>0.35008818342151676</v>
-      </c>
-      <c r="G60" s="3">
-        <f>(D60/D59)/(A60/A59)</f>
         <v>0.29342636797649652</v>
       </c>
     </row>
@@ -8758,27 +9217,27 @@
         <v>100</v>
       </c>
       <c r="B61" s="3">
+        <f t="shared" si="7"/>
+        <v>32.439999999999998</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="8"/>
+        <v>18.649999999999999</v>
+      </c>
+      <c r="D61" s="1">
+        <f t="shared" si="9"/>
+        <v>38.409999999999997</v>
+      </c>
+      <c r="E61" s="3">
+        <f t="shared" si="3"/>
+        <v>0.45851590106007062</v>
+      </c>
+      <c r="F61" s="3">
         <f t="shared" si="4"/>
-        <v>32.439999999999998</v>
-      </c>
-      <c r="C61">
+        <v>0.46977329974811077</v>
+      </c>
+      <c r="G61" s="3">
         <f t="shared" si="5"/>
-        <v>18.649999999999999</v>
-      </c>
-      <c r="D61" s="1">
-        <f t="shared" si="6"/>
-        <v>38.409999999999997</v>
-      </c>
-      <c r="E61" s="3">
-        <f>(B61/B60)/(A61/A60)</f>
-        <v>0.45851590106007062</v>
-      </c>
-      <c r="F61" s="3">
-        <f>(C61/C60)/(A61/A60)</f>
-        <v>0.46977329974811077</v>
-      </c>
-      <c r="G61" s="3">
-        <f>(D61/D60)/(A61/A60)</f>
         <v>0.24036295369211511</v>
       </c>
     </row>
@@ -8787,27 +9246,27 @@
         <v>200</v>
       </c>
       <c r="B62" s="3">
+        <f t="shared" si="7"/>
+        <v>60.280000000000001</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="8"/>
+        <v>25.100000000000001</v>
+      </c>
+      <c r="D62" s="1">
+        <f t="shared" si="9"/>
+        <v>48.710000000000001</v>
+      </c>
+      <c r="E62" s="3">
+        <f t="shared" si="3"/>
+        <v>0.92909987669543781</v>
+      </c>
+      <c r="F62" s="3">
         <f t="shared" si="4"/>
-        <v>60.280000000000001</v>
-      </c>
-      <c r="C62">
+        <v>0.67292225201072398</v>
+      </c>
+      <c r="G62" s="3">
         <f t="shared" si="5"/>
-        <v>25.100000000000001</v>
-      </c>
-      <c r="D62" s="1">
-        <f t="shared" si="6"/>
-        <v>48.710000000000001</v>
-      </c>
-      <c r="E62" s="3">
-        <f>(B62/B61)/(A62/A61)</f>
-        <v>0.92909987669543781</v>
-      </c>
-      <c r="F62" s="3">
-        <f>(C62/C61)/(A62/A61)</f>
-        <v>0.67292225201072398</v>
-      </c>
-      <c r="G62" s="3">
-        <f>(D62/D61)/(A62/A61)</f>
         <v>0.63407966675344973</v>
       </c>
     </row>
@@ -8852,15 +9311,15 @@
         <v>1</v>
       </c>
       <c r="B66" s="5">
-        <f t="shared" ref="B66:B70" si="7">D32</f>
+        <f t="shared" ref="B66:B70" si="10">D32</f>
         <v>13.710000000000001</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C70" si="8">D37</f>
+        <f t="shared" ref="C66:C70" si="11">D37</f>
         <v>8.9700000000000006</v>
       </c>
       <c r="D66" s="1">
-        <f t="shared" ref="D66:D70" si="9">D42</f>
+        <f t="shared" ref="D66:D70" si="12">D42</f>
         <v>28.300000000000001</v>
       </c>
       <c r="E66" s="1" t="s">
@@ -8878,27 +9337,27 @@
         <v>5</v>
       </c>
       <c r="B67" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>17.289999999999999</v>
       </c>
       <c r="C67">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>9.3100000000000005</v>
       </c>
       <c r="D67" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>29.93</v>
       </c>
       <c r="E67" s="3">
-        <f>(B67/B66)/(A67/A66)</f>
+        <f t="shared" si="3"/>
         <v>0.25222465353756379</v>
       </c>
       <c r="F67" s="3">
-        <f>(C67/C66)/(A67/A66)</f>
+        <f t="shared" si="4"/>
         <v>0.20758082497212932</v>
       </c>
       <c r="G67" s="3">
-        <f>(D67/D66)/(A67/A66)</f>
+        <f t="shared" si="5"/>
         <v>0.21151943462897527</v>
       </c>
     </row>
@@ -8907,27 +9366,27 @@
         <v>20</v>
       </c>
       <c r="B68" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>22.579999999999998</v>
       </c>
       <c r="C68">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>11.380000000000001</v>
       </c>
       <c r="D68" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>32.590000000000003</v>
       </c>
       <c r="E68" s="3">
-        <f>(B68/B67)/(A68/A67)</f>
+        <f t="shared" si="3"/>
         <v>0.32648930017351069</v>
       </c>
       <c r="F68" s="3">
-        <f>(C68/C67)/(A68/A67)</f>
+        <f t="shared" si="4"/>
         <v>0.30558539205155749</v>
       </c>
       <c r="G68" s="3">
-        <f>(D68/D67)/(A68/A67)</f>
+        <f t="shared" si="5"/>
         <v>0.27221850985633145</v>
       </c>
     </row>
@@ -8936,27 +9395,27 @@
         <v>100</v>
       </c>
       <c r="B69" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>46.789999999999999</v>
       </c>
       <c r="C69">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>21.370000000000001</v>
       </c>
       <c r="D69" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>36.579999999999998</v>
       </c>
       <c r="E69" s="3">
-        <f>(B69/B68)/(A69/A68)</f>
+        <f t="shared" si="3"/>
         <v>0.41443755535872456</v>
       </c>
       <c r="F69" s="3">
-        <f>(C69/C68)/(A69/A68)</f>
+        <f t="shared" si="4"/>
         <v>0.37557117750439367</v>
       </c>
       <c r="G69" s="3">
-        <f>(D69/D68)/(A69/A68)</f>
+        <f t="shared" si="5"/>
         <v>0.22448603866216627</v>
       </c>
     </row>
@@ -8965,23 +9424,23 @@
         <v>200</v>
       </c>
       <c r="B70" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>81.769999999999996</v>
       </c>
       <c r="C70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>36.719999999999999</v>
       </c>
       <c r="D70" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>42.340000000000003</v>
       </c>
       <c r="E70" s="3">
-        <f>(B70/B69)/(A70/A69)</f>
+        <f t="shared" si="3"/>
         <v>0.87379782004701856</v>
       </c>
       <c r="F70" s="3">
-        <f>(C70/C69)/(A70/A69)</f>
+        <f t="shared" si="4"/>
         <v>0.85914833879270003</v>
       </c>
       <c r="G70" s="3">
@@ -9068,7 +9527,7 @@
       <c r="C4" s="6">
         <v>20</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="7">
         <v>100.56999999999999</v>
       </c>
     </row>
@@ -9082,7 +9541,7 @@
       <c r="C5" s="6">
         <v>100</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="7">
         <v>516.97000000000003</v>
       </c>
     </row>
@@ -9096,7 +9555,7 @@
       <c r="C6" s="6">
         <v>200</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="8">
         <v>1009.01</v>
       </c>
     </row>
@@ -9292,7 +9751,7 @@
       <c r="C20" s="6">
         <v>100</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="7">
         <v>204.75999999999999</v>
       </c>
     </row>
@@ -9306,7 +9765,7 @@
       <c r="C21" s="6">
         <v>200</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="7">
         <v>417.10000000000002</v>
       </c>
     </row>
@@ -9681,13 +10140,13 @@
       <c r="D49" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="E49" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F49" s="11" t="s">
+      <c r="F49" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G49" s="11" t="s">
+      <c r="G49" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -9696,15 +10155,15 @@
         <v>1</v>
       </c>
       <c r="B50" s="3">
-        <f t="shared" ref="B50:B54" si="10">D2</f>
+        <f t="shared" ref="B50:B54" si="13">D2</f>
         <v>8.0199999999999996</v>
       </c>
       <c r="C50" s="1">
-        <f t="shared" ref="C50:C52" si="11">D7</f>
+        <f t="shared" ref="C50:C52" si="14">D7</f>
         <v>4.3399999999999999</v>
       </c>
       <c r="D50" s="1">
-        <f t="shared" ref="D50:D54" si="12">D12</f>
+        <f t="shared" ref="D50:D54" si="15">D12</f>
         <v>30.84</v>
       </c>
       <c r="E50" s="1" t="s">
@@ -9722,27 +10181,27 @@
         <v>5</v>
       </c>
       <c r="B51" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>26.100000000000001</v>
       </c>
       <c r="C51" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>13.359999999999999</v>
       </c>
       <c r="D51" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>35.979999999999997</v>
       </c>
       <c r="E51" s="3">
-        <f>(B51/B50)/(A51/A50)</f>
+        <f t="shared" ref="E51:E70" si="16">(B51/B50)/(A51/A50)</f>
         <v>0.65087281795511231</v>
       </c>
       <c r="F51" s="3">
-        <f>(C51/C50)/(A51/A50)</f>
+        <f t="shared" ref="F51:F70" si="17">(C51/C50)/(A51/A50)</f>
         <v>0.61566820276497691</v>
       </c>
       <c r="G51" s="3">
-        <f>(D51/D50)/(A51/A50)</f>
+        <f t="shared" ref="G51:G70" si="18">(D51/D50)/(A51/A50)</f>
         <v>0.23333333333333331</v>
       </c>
     </row>
@@ -9751,27 +10210,27 @@
         <v>20</v>
       </c>
       <c r="B52" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>100.56999999999999</v>
       </c>
       <c r="C52" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>46.380000000000003</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>56.890000000000001</v>
       </c>
       <c r="E52" s="3">
-        <f>(B52/B51)/(A52/A51)</f>
+        <f t="shared" si="16"/>
         <v>0.96331417624521065</v>
       </c>
       <c r="F52" s="3">
-        <f>(C52/C51)/(A52/A51)</f>
+        <f t="shared" si="17"/>
         <v>0.8678892215568863</v>
       </c>
       <c r="G52" s="3">
-        <f>(D52/D51)/(A52/A51)</f>
+        <f t="shared" si="18"/>
         <v>0.39528904947192889</v>
       </c>
     </row>
@@ -9780,27 +10239,27 @@
         <v>100</v>
       </c>
       <c r="B53" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>516.97000000000003</v>
       </c>
       <c r="C53" s="1">
-        <f t="shared" ref="C53:C54" si="13">D10</f>
+        <f t="shared" ref="C53:C54" si="19">D10</f>
         <v>243.68000000000001</v>
       </c>
       <c r="D53" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>228.63</v>
       </c>
       <c r="E53" s="3">
-        <f>(B53/B52)/(A53/A52)</f>
+        <f t="shared" si="16"/>
         <v>1.0280799443173909</v>
       </c>
       <c r="F53" s="3">
-        <f>(C53/C52)/(A53/A52)</f>
+        <f t="shared" si="17"/>
         <v>1.0507977576541614</v>
       </c>
       <c r="G53" s="3">
-        <f>(D53/D52)/(A53/A52)</f>
+        <f t="shared" si="18"/>
         <v>0.80376164528036553</v>
       </c>
     </row>
@@ -9809,27 +10268,27 @@
         <v>200</v>
       </c>
       <c r="B54" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1009.01</v>
       </c>
       <c r="C54" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>506.67000000000002</v>
       </c>
       <c r="D54" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>425.89699999999999</v>
       </c>
       <c r="E54" s="3">
-        <f>(B54/B53)/(A54/A53)</f>
+        <f t="shared" si="16"/>
         <v>0.9758883494206626</v>
       </c>
       <c r="F54" s="3">
-        <f>(C54/C53)/(A54/A53)</f>
+        <f t="shared" si="17"/>
         <v>1.0396216349310572</v>
       </c>
       <c r="G54" s="3">
-        <f>(D54/D53)/(A54/A53)</f>
+        <f t="shared" si="18"/>
         <v>0.93141101342780908</v>
       </c>
     </row>
@@ -9880,15 +10339,15 @@
         <v>1</v>
       </c>
       <c r="B58" s="3">
-        <f t="shared" ref="B58:B62" si="14">D17</f>
+        <f t="shared" ref="B58:B62" si="20">D17</f>
         <v>8.8900000000000006</v>
       </c>
       <c r="C58" s="6">
-        <f t="shared" ref="C58:C62" si="15">D22</f>
+        <f t="shared" ref="C58:C62" si="21">D22</f>
         <v>4.6100000000000003</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" ref="D58:D62" si="16">D27</f>
+        <f t="shared" ref="D58:D62" si="22">D27</f>
         <v>26.09</v>
       </c>
       <c r="E58" s="1" t="s">
@@ -9906,27 +10365,27 @@
         <v>5</v>
       </c>
       <c r="B59" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>18.059999999999999</v>
       </c>
       <c r="C59" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>7.0599999999999996</v>
       </c>
       <c r="D59" s="1">
+        <f t="shared" si="22"/>
+        <v>38.119999999999997</v>
+      </c>
+      <c r="E59" s="3">
         <f t="shared" si="16"/>
-        <v>38.119999999999997</v>
-      </c>
-      <c r="E59" s="3">
-        <f>(B59/B58)/(A59/A58)</f>
         <v>0.40629921259842516</v>
       </c>
       <c r="F59" s="3">
-        <f>(C59/C58)/(A59/A58)</f>
+        <f t="shared" si="17"/>
         <v>0.30629067245119301</v>
       </c>
       <c r="G59" s="3">
-        <f>(D59/D58)/(A59/A58)</f>
+        <f t="shared" si="18"/>
         <v>0.29221924108853969</v>
       </c>
     </row>
@@ -9935,27 +10394,27 @@
         <v>20</v>
       </c>
       <c r="B60" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>49.82</v>
       </c>
       <c r="C60" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>10.25</v>
       </c>
       <c r="D60" s="1">
+        <f t="shared" si="22"/>
+        <v>67.359999999999999</v>
+      </c>
+      <c r="E60" s="3">
         <f t="shared" si="16"/>
-        <v>67.359999999999999</v>
-      </c>
-      <c r="E60" s="3">
-        <f>(B60/B59)/(A60/A59)</f>
         <v>0.68964562569213739</v>
       </c>
       <c r="F60" s="3">
-        <f>(C60/C59)/(A60/A59)</f>
+        <f t="shared" si="17"/>
         <v>0.36296033994334281</v>
       </c>
       <c r="G60" s="3">
-        <f>(D60/D59)/(A60/A59)</f>
+        <f t="shared" si="18"/>
         <v>0.44176285414480593</v>
       </c>
     </row>
@@ -9964,27 +10423,27 @@
         <v>100</v>
       </c>
       <c r="B61" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>204.75999999999999</v>
       </c>
       <c r="C61" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>44.840000000000003</v>
       </c>
       <c r="D61" s="1">
+        <f t="shared" si="22"/>
+        <v>127.29000000000001</v>
+      </c>
+      <c r="E61" s="3">
         <f t="shared" si="16"/>
-        <v>127.29000000000001</v>
-      </c>
-      <c r="E61" s="3">
-        <f>(B61/B60)/(A61/A60)</f>
         <v>0.82199919710959457</v>
       </c>
       <c r="F61" s="3">
-        <f>(C61/C60)/(A61/A60)</f>
+        <f t="shared" si="17"/>
         <v>0.87492682926829279</v>
       </c>
       <c r="G61" s="3">
-        <f>(D61/D60)/(A61/A60)</f>
+        <f t="shared" si="18"/>
         <v>0.37793942992874113</v>
       </c>
     </row>
@@ -9993,27 +10452,27 @@
         <v>200</v>
       </c>
       <c r="B62" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>417.10000000000002</v>
       </c>
       <c r="C62" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>89.969999999999999</v>
       </c>
       <c r="D62" s="1">
+        <f t="shared" si="22"/>
+        <v>225.02000000000001</v>
+      </c>
+      <c r="E62" s="3">
         <f t="shared" si="16"/>
-        <v>225.02000000000001</v>
-      </c>
-      <c r="E62" s="3">
-        <f>(B62/B61)/(A62/A61)</f>
         <v>1.0185094745067398</v>
       </c>
       <c r="F62" s="3">
-        <f>(C62/C61)/(A62/A61)</f>
+        <f t="shared" si="17"/>
         <v>1.0032337198929526</v>
       </c>
       <c r="G62" s="3">
-        <f>(D62/D61)/(A62/A61)</f>
+        <f t="shared" si="18"/>
         <v>0.88388718673894262</v>
       </c>
     </row>
@@ -10065,15 +10524,15 @@
         <v>1</v>
       </c>
       <c r="B66" s="5">
-        <f t="shared" ref="B66:B70" si="17">D32</f>
+        <f t="shared" ref="B66:B70" si="23">D32</f>
         <v>10.18</v>
       </c>
       <c r="C66" s="6">
-        <f t="shared" ref="C66:C70" si="18">D37</f>
+        <f t="shared" ref="C66:C70" si="24">D37</f>
         <v>7.1500000000000004</v>
       </c>
       <c r="D66" s="1">
-        <f t="shared" ref="D66:D70" si="19">D42</f>
+        <f t="shared" ref="D66:D70" si="25">D42</f>
         <v>75.829999999999998</v>
       </c>
       <c r="E66" s="1" t="s">
@@ -10091,28 +10550,28 @@
         <v>5</v>
       </c>
       <c r="B67" s="5">
+        <f t="shared" si="23"/>
+        <v>11.51</v>
+      </c>
+      <c r="C67" s="6">
+        <f t="shared" si="24"/>
+        <v>7.3899999999999997</v>
+      </c>
+      <c r="D67" s="1">
+        <f t="shared" si="25"/>
+        <v>16.510000000000002</v>
+      </c>
+      <c r="E67" s="3">
+        <f t="shared" si="16"/>
+        <v>0.22612966601178783</v>
+      </c>
+      <c r="F67" s="3">
         <f t="shared" si="17"/>
-        <v>11.51</v>
-      </c>
-      <c r="C67" s="6">
+        <v>0.20671328671328668</v>
+      </c>
+      <c r="G67" s="3">
         <f t="shared" si="18"/>
-        <v>7.3899999999999997</v>
-      </c>
-      <c r="D67" s="1">
-        <f t="shared" si="19"/>
-        <v>16.510000000000002</v>
-      </c>
-      <c r="E67" s="3">
-        <f>(B67/B66)/(A67/A66)</f>
-        <v>0.22612966601178783</v>
-      </c>
-      <c r="F67" s="3">
-        <f>(C67/C66)/(A67/A66)</f>
-        <v>0.20671328671328668</v>
-      </c>
-      <c r="G67" s="3">
-        <f>(D67/D66)/(A67/A66)</f>
-        <v>0.043544771198734018</v>
+        <v>4.3544771198734018e-002</v>
       </c>
     </row>
     <row r="68" ht="14.25">
@@ -10120,27 +10579,27 @@
         <v>20</v>
       </c>
       <c r="B68" s="5">
+        <f t="shared" si="23"/>
+        <v>12.710000000000001</v>
+      </c>
+      <c r="C68" s="6">
+        <f t="shared" si="24"/>
+        <v>7.0300000000000002</v>
+      </c>
+      <c r="D68" s="1">
+        <f t="shared" si="25"/>
+        <v>17.129999999999999</v>
+      </c>
+      <c r="E68" s="3">
+        <f t="shared" si="16"/>
+        <v>0.27606429192006954</v>
+      </c>
+      <c r="F68" s="3">
         <f t="shared" si="17"/>
-        <v>12.710000000000001</v>
-      </c>
-      <c r="C68" s="6">
+        <v>0.23782138024357241</v>
+      </c>
+      <c r="G68" s="3">
         <f t="shared" si="18"/>
-        <v>7.0300000000000002</v>
-      </c>
-      <c r="D68" s="1">
-        <f t="shared" si="19"/>
-        <v>17.129999999999999</v>
-      </c>
-      <c r="E68" s="3">
-        <f>(B68/B67)/(A68/A67)</f>
-        <v>0.27606429192006954</v>
-      </c>
-      <c r="F68" s="3">
-        <f>(C68/C67)/(A68/A67)</f>
-        <v>0.23782138024357241</v>
-      </c>
-      <c r="G68" s="3">
-        <f>(D68/D67)/(A68/A67)</f>
         <v>0.25938824954572981</v>
       </c>
     </row>
@@ -10149,27 +10608,27 @@
         <v>100</v>
       </c>
       <c r="B69" s="5">
+        <f t="shared" si="23"/>
+        <v>12.68</v>
+      </c>
+      <c r="C69" s="6">
+        <f t="shared" si="24"/>
+        <v>6.9400000000000004</v>
+      </c>
+      <c r="D69" s="1">
+        <f t="shared" si="25"/>
+        <v>15.59</v>
+      </c>
+      <c r="E69" s="3">
+        <f t="shared" si="16"/>
+        <v>0.1995279307631786</v>
+      </c>
+      <c r="F69" s="3">
         <f t="shared" si="17"/>
-        <v>12.68</v>
-      </c>
-      <c r="C69" s="6">
+        <v>0.19743954480796586</v>
+      </c>
+      <c r="G69" s="3">
         <f t="shared" si="18"/>
-        <v>6.9400000000000004</v>
-      </c>
-      <c r="D69" s="1">
-        <f t="shared" si="19"/>
-        <v>15.59</v>
-      </c>
-      <c r="E69" s="3">
-        <f>(B69/B68)/(A69/A68)</f>
-        <v>0.1995279307631786</v>
-      </c>
-      <c r="F69" s="3">
-        <f>(C69/C68)/(A69/A68)</f>
-        <v>0.19743954480796586</v>
-      </c>
-      <c r="G69" s="3">
-        <f>(D69/D68)/(A69/A68)</f>
         <v>0.18201984821949796</v>
       </c>
     </row>
@@ -10178,27 +10637,27 @@
         <v>200</v>
       </c>
       <c r="B70" s="5">
+        <f t="shared" si="23"/>
+        <v>12.67</v>
+      </c>
+      <c r="C70" s="6">
+        <f t="shared" si="24"/>
+        <v>7.1200000000000001</v>
+      </c>
+      <c r="D70" s="1">
+        <f t="shared" si="25"/>
+        <v>17.760000000000002</v>
+      </c>
+      <c r="E70" s="3">
+        <f t="shared" si="16"/>
+        <v>0.49960567823343849</v>
+      </c>
+      <c r="F70" s="3">
         <f t="shared" si="17"/>
-        <v>12.67</v>
-      </c>
-      <c r="C70" s="6">
+        <v>0.51296829971181557</v>
+      </c>
+      <c r="G70" s="3">
         <f t="shared" si="18"/>
-        <v>7.1200000000000001</v>
-      </c>
-      <c r="D70" s="1">
-        <f t="shared" si="19"/>
-        <v>17.760000000000002</v>
-      </c>
-      <c r="E70" s="3">
-        <f>(B70/B69)/(A70/A69)</f>
-        <v>0.49960567823343849</v>
-      </c>
-      <c r="F70" s="3">
-        <f>(C70/C69)/(A70/A69)</f>
-        <v>0.51296829971181557</v>
-      </c>
-      <c r="G70" s="3">
-        <f>(D70/D69)/(A70/A69)</f>
         <v>0.56959589480436179</v>
       </c>
     </row>

</xml_diff>